<commit_message>
Huge update: fin #6-7.7
rigorous date treatment, returns calc, new features - delay, price change in the delay, better filtering methods - addv/low/no price n vol/etc. hella stoked
</commit_message>
<xml_diff>
--- a/failed_log2.xlsx
+++ b/failed_log2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John DeForest\Desktop\stonx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C0ACBB-7226-44D5-9AC2-7FED305BEDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D089A57-722B-40E2-9C80-199603715D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32625" yWindow="3855" windowWidth="17280" windowHeight="10515" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
+    <workbookView xWindow="2208" yWindow="1056" windowWidth="17280" windowHeight="10512" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
   </bookViews>
   <sheets>
     <sheet name="failed_log2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={81845068-A864-422B-A307-D209ED86063D}</author>
+    <author>tc={87EC06C1-C95E-4B45-B805-4D4BCEE2B9EE}</author>
     <author>tc={41293392-54A1-4296-96FD-EDB13FBD4F4E}</author>
+    <author>tc={CB4462E8-6D40-43DF-871C-DAA05325856A}</author>
   </authors>
   <commentList>
     <comment ref="K1" authorId="0" shapeId="0" xr:uid="{81845068-A864-422B-A307-D209ED86063D}">
@@ -49,7 +51,15 @@
     F is full name and ticker / T is just ticker / N is just name</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" shapeId="0" xr:uid="{41293392-54A1-4296-96FD-EDB13FBD4F4E}">
+    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{87EC06C1-C95E-4B45-B805-4D4BCEE2B9EE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    (does ticker/company exist/have current stock records findable?</t>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="2" shapeId="0" xr:uid="{41293392-54A1-4296-96FD-EDB13FBD4F4E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -57,12 +67,22 @@
     G = google search only, It = investing.com search bar ticker, in = ‘ full name</t>
       </text>
     </comment>
+    <comment ref="G62" authorId="3" shapeId="0" xr:uid="{CB4462E8-6D40-43DF-871C-DAA05325856A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Double check this manually from the openinsider info...
+Reply:
+    Was like 6.70$ at that dateish</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="232">
   <si>
     <t>ticker</t>
   </si>
@@ -728,6 +748,36 @@
   </si>
   <si>
     <t>https://www.investing.com/equities/absolute-software-corp-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/transcept-pharmaceuticals-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/chimerix-inc-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/alexander-energy-ltd-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/air-transport-service-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/amerco-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/harpoon-therapeutics-inc-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/aziyo-biologics-inc-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/intevac-historical-data</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/american-equity-holdings-historical-data</t>
+  </si>
+  <si>
+    <t>Exists?</t>
   </si>
 </sst>
 </file>
@@ -737,7 +787,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,8 +930,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1079,6 +1135,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1241,7 +1303,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1250,6 +1312,8 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1684,18 +1748,27 @@
   <threadedComment ref="K1" dT="2025-07-31T19:05:13.73" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{F194CF49-579B-4228-B62E-BFBB6E705764}" parentId="{81845068-A864-422B-A307-D209ED86063D}">
     <text>F is full name and ticker / T is just ticker / N is just name</text>
   </threadedComment>
-  <threadedComment ref="X1" dT="2025-07-31T18:20:10.90" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{41293392-54A1-4296-96FD-EDB13FBD4F4E}">
+  <threadedComment ref="T1" dT="2025-08-03T05:12:30.98" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{87EC06C1-C95E-4B45-B805-4D4BCEE2B9EE}">
+    <text>(does ticker/company exist/have current stock records findable?</text>
+  </threadedComment>
+  <threadedComment ref="Y1" dT="2025-07-31T18:20:10.90" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{41293392-54A1-4296-96FD-EDB13FBD4F4E}">
     <text>G = google search only, It = investing.com search bar ticker, in = ‘ full name</text>
+  </threadedComment>
+  <threadedComment ref="G62" dT="2025-08-03T05:02:25.58" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{CB4462E8-6D40-43DF-871C-DAA05325856A}">
+    <text>Double check this manually from the openinsider info...</text>
+  </threadedComment>
+  <threadedComment ref="G62" dT="2025-08-03T05:03:15.40" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{93D35AF8-C021-46EF-BC51-950FAF86D9AC}" parentId="{CB4462E8-6D40-43DF-871C-DAA05325856A}">
+    <text>Was like 6.70$ at that dateish</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10141A12-633E-46F9-B8A5-FB31F61A7B2A}">
-  <dimension ref="A1:AG66"/>
+  <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1717,13 +1790,13 @@
     <col min="16" max="16" width="7.77734375" customWidth="1"/>
     <col min="17" max="17" width="5.77734375" customWidth="1"/>
     <col min="18" max="18" width="5.88671875" customWidth="1"/>
-    <col min="19" max="19" width="5.77734375" customWidth="1"/>
-    <col min="20" max="20" width="45.109375" customWidth="1"/>
-    <col min="21" max="21" width="31.44140625" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" customWidth="1"/>
+    <col min="19" max="20" width="5.77734375" customWidth="1"/>
+    <col min="21" max="21" width="45.109375" customWidth="1"/>
+    <col min="22" max="22" width="31.44140625" customWidth="1"/>
+    <col min="23" max="23" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1782,49 +1855,52 @@
         <v>176</v>
       </c>
       <c r="T1" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>161</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>163</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>158</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>11</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>16</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1855,11 +1931,11 @@
       <c r="L2" t="s">
         <v>162</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1918,11 +1994,8 @@
       <c r="S3" t="s">
         <v>166</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>178</v>
-      </c>
-      <c r="Y3">
-        <v>1</v>
       </c>
       <c r="Z3">
         <v>1</v>
@@ -1930,8 +2003,11 @@
       <c r="AA3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AB3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1987,23 +2063,23 @@
       <c r="S4" t="s">
         <v>166</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>159</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>160</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
       </c>
       <c r="Z4">
         <v>0</v>
       </c>
       <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -2056,11 +2132,11 @@
       <c r="S5" t="s">
         <v>166</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -2092,11 +2168,11 @@
         <f t="shared" si="0"/>
         <v>Central Valley Community Bancorp CVCY</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -2128,39 +2204,39 @@
         <f t="shared" si="0"/>
         <v>Beacon Roofing Supply Inc BECN</v>
       </c>
-      <c r="T7" s="7" t="s">
+      <c r="U7" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="U7" s="7"/>
-      <c r="Y7">
-        <v>0</v>
-      </c>
+      <c r="V7" s="7"/>
       <c r="Z7">
         <v>0</v>
       </c>
       <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
         <v>1</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>32</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>33</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>34</v>
       </c>
-      <c r="AE7">
+      <c r="AF7">
         <v>0</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>1</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AH7" s="2">
         <v>45776</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2195,11 +2271,11 @@
       <c r="S8" t="s">
         <v>187</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -2234,17 +2310,17 @@
       <c r="S9" t="s">
         <v>187</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>183</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>39</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2279,17 +2355,17 @@
       <c r="S10" t="s">
         <v>187</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>184</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>1</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <v>0.26153846200000003</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2321,14 +2397,14 @@
         <f t="shared" si="0"/>
         <v>Athena Gold Corp AHNR</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>1.5</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>0.3125</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -2360,14 +2436,14 @@
         <f t="shared" si="0"/>
         <v>Ault Alliance, Inc. AULT</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>2</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>0.44444444399999999</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2402,17 +2478,17 @@
       <c r="S13" t="s">
         <v>187</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>185</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>2.5</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>0.45161290300000001</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -2453,20 +2529,20 @@
       <c r="S14" t="s">
         <v>166</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>186</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
       </c>
       <c r="Z14">
         <v>0</v>
       </c>
       <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2498,11 +2574,11 @@
         <f t="shared" si="0"/>
         <v>Fusion Acquisition Corp. II FSNB</v>
       </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2534,11 +2610,11 @@
         <f t="shared" si="0"/>
         <v>Chembio Diagnostics, Inc. CEMI</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2570,11 +2646,11 @@
         <f t="shared" si="0"/>
         <v>Community Trust Bancorp Inc /Ky/ QGNC</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -2606,11 +2682,11 @@
         <f t="shared" si="0"/>
         <v>William Penn Bancorporation WMPN</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -2642,11 +2718,11 @@
         <f t="shared" si="0"/>
         <v>Stronghold Digital Mining, Inc. SDIG</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -2679,7 +2755,7 @@
         <v>Cyclo Therapeutics, Inc. CYTH</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -2711,26 +2787,26 @@
         <f t="shared" si="0"/>
         <v>Augmedix, Inc. AUGX</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>192</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="AD21" t="s">
         <v>65</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>34</v>
       </c>
-      <c r="AE21">
+      <c r="AF21">
         <v>0</v>
       </c>
-      <c r="AF21">
+      <c r="AG21">
         <v>1</v>
       </c>
-      <c r="AG21" s="2">
+      <c r="AH21" s="2">
         <v>45567</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -2777,14 +2853,14 @@
       <c r="S22" t="s">
         <v>166</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>195</v>
       </c>
-      <c r="U22" t="s">
+      <c r="V22" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -2817,7 +2893,7 @@
         <v>Verde Bio Holdings, Inc. VBHI</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -2849,11 +2925,11 @@
         <f t="shared" si="0"/>
         <v>Ambrx Biopharma Inc. AMAM</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2894,11 +2970,11 @@
       <c r="S25" t="s">
         <v>166</v>
       </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2930,11 +3006,11 @@
         <f t="shared" si="0"/>
         <v>Joann Inc. JOAN</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -2967,7 +3043,7 @@
         <v>Oncternal Therapeutics, Inc. ONCT</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -3000,7 +3076,7 @@
         <v>Malachite Innovations, Inc. MLCT</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -3033,7 +3109,7 @@
         <v>United States Basketball League Inc USBL</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -3065,20 +3141,20 @@
         <f t="shared" si="0"/>
         <v>Safeguard Scientifics Inc SFE</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>198</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>84</v>
-      </c>
-      <c r="Z30">
-        <v>1</v>
       </c>
       <c r="AA30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AB30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -3110,11 +3186,11 @@
         <f t="shared" si="0"/>
         <v>Patriot Transportation Holding, Inc. PATI</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -3146,14 +3222,14 @@
         <f t="shared" si="0"/>
         <v>Monterey Innovation Acquisition Corp MTRY</v>
       </c>
-      <c r="Y32">
-        <v>0</v>
-      </c>
       <c r="Z32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -3186,7 +3262,7 @@
         <v>Obseva Sa OBSV</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -3227,11 +3303,11 @@
       <c r="S34" t="s">
         <v>166</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>93</v>
       </c>
@@ -3272,11 +3348,11 @@
       <c r="S35" t="s">
         <v>166</v>
       </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -3308,11 +3384,11 @@
         <f t="shared" si="0"/>
         <v>Corner Growth Acquisition Corp. COOL</v>
       </c>
-      <c r="T36" t="s">
+      <c r="U36" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -3344,11 +3420,11 @@
         <f t="shared" si="0"/>
         <v>Pardes Biosciences, Inc. PRDS</v>
       </c>
-      <c r="T37" t="s">
+      <c r="U37" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -3381,7 +3457,7 @@
         <v>Metaworks Platforms, Inc. MWRK</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -3413,11 +3489,11 @@
         <f t="shared" si="0"/>
         <v>Malvern Bancorp, Inc. MLVF</v>
       </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -3458,11 +3534,11 @@
       <c r="S40" t="s">
         <v>166</v>
       </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -3495,7 +3571,7 @@
         <v>Sarcos Technology &amp; Robotics Corp STRC</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -3527,11 +3603,11 @@
         <f t="shared" si="0"/>
         <v>Curo Group Holdings Corp. CURO</v>
       </c>
-      <c r="T42" t="s">
+      <c r="U42" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -3563,17 +3639,17 @@
         <f t="shared" si="0"/>
         <v>Bird Global, Inc. BRDS</v>
       </c>
-      <c r="Y43">
-        <v>0</v>
-      </c>
       <c r="Z43">
         <v>0</v>
       </c>
       <c r="AA43">
+        <v>0</v>
+      </c>
+      <c r="AB43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>111</v>
       </c>
@@ -3605,11 +3681,11 @@
         <f t="shared" si="0"/>
         <v>Trailblazer Merger Corp I TBMCU</v>
       </c>
-      <c r="T44" t="s">
+      <c r="U44" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>113</v>
       </c>
@@ -3641,11 +3717,11 @@
         <f t="shared" si="0"/>
         <v>Codorus Valley Bancorp Inc CVLY</v>
       </c>
-      <c r="T45" t="s">
+      <c r="U45" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>115</v>
       </c>
@@ -3677,11 +3753,11 @@
         <f t="shared" si="0"/>
         <v>Activision Blizzard, Inc. ATVI</v>
       </c>
-      <c r="T46" t="s">
+      <c r="U46" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -3713,17 +3789,17 @@
         <f t="shared" si="0"/>
         <v>Profrac Holding Corp. PFHC</v>
       </c>
-      <c r="T47" t="s">
+      <c r="U47" t="s">
         <v>210</v>
       </c>
-      <c r="U47" t="s">
+      <c r="V47" t="s">
         <v>219</v>
       </c>
-      <c r="V47" t="s">
+      <c r="W47" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -3755,17 +3831,17 @@
         <f t="shared" si="0"/>
         <v>Glatfelter Corp GLT</v>
       </c>
-      <c r="T48" t="s">
+      <c r="U48" t="s">
         <v>211</v>
       </c>
-      <c r="U48" t="s">
+      <c r="V48" t="s">
         <v>212</v>
       </c>
-      <c r="V48" t="s">
+      <c r="W48" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>121</v>
       </c>
@@ -3797,11 +3873,11 @@
         <f t="shared" si="0"/>
         <v>Adams Resources &amp; Energy, Inc. AE</v>
       </c>
-      <c r="T49" t="s">
+      <c r="U49" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -3833,11 +3909,11 @@
         <f t="shared" si="0"/>
         <v>Terrascend Corp. TRSSF</v>
       </c>
-      <c r="T50" t="s">
+      <c r="U50" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>125</v>
       </c>
@@ -3869,11 +3945,11 @@
         <f t="shared" si="0"/>
         <v>Sentinel Energy Services Inc. STNL</v>
       </c>
-      <c r="T51" t="s">
+      <c r="U51" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>127</v>
       </c>
@@ -3905,23 +3981,23 @@
         <f t="shared" si="0"/>
         <v>Dice Therapeutics, Inc. DICE</v>
       </c>
-      <c r="T52" t="s">
+      <c r="U52" t="s">
         <v>218</v>
-      </c>
-      <c r="Y52">
-        <v>0</v>
       </c>
       <c r="Z52">
         <v>0</v>
       </c>
       <c r="AA52">
+        <v>0</v>
+      </c>
+      <c r="AB52">
         <v>1</v>
       </c>
-      <c r="AB52" t="s">
+      <c r="AC52" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>130</v>
       </c>
@@ -3953,11 +4029,11 @@
         <f t="shared" si="0"/>
         <v>Miromatrix Medical Inc. MIRO</v>
       </c>
-      <c r="T53" t="s">
+      <c r="U53" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -3989,11 +4065,11 @@
         <f t="shared" si="0"/>
         <v>Absolute Software Corp ABST</v>
       </c>
-      <c r="T54" t="s">
+      <c r="U54" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -4026,7 +4102,7 @@
         <v>Know Labs, Inc. KNWN</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -4058,8 +4134,11 @@
         <f t="shared" si="0"/>
         <v>Paratek Pharmaceuticals, Inc. PRTK</v>
       </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U56" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -4091,8 +4170,8 @@
         <f t="shared" si="0"/>
         <v>Chimerix Inc CMRX</v>
       </c>
-      <c r="Y57">
-        <v>0</v>
+      <c r="U57" t="s">
+        <v>223</v>
       </c>
       <c r="Z57">
         <v>0</v>
@@ -4100,8 +4179,11 @@
       <c r="AA57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AB57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -4133,8 +4215,11 @@
         <f t="shared" si="0"/>
         <v>Fisker Inc./de FSR</v>
       </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U58" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>142</v>
       </c>
@@ -4167,7 +4252,7 @@
         <v>Superior Drilling Products, Inc. SDPI</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>144</v>
       </c>
@@ -4199,8 +4284,11 @@
         <f t="shared" si="0"/>
         <v>Air Transport Services Group, Inc. ATSG</v>
       </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U60" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>146</v>
       </c>
@@ -4232,8 +4320,11 @@
         <f t="shared" si="0"/>
         <v>U-Haul Holding Co /Nv/ UHALU</v>
       </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U61" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>148</v>
       </c>
@@ -4252,7 +4343,7 @@
       <c r="F62" t="s">
         <v>21</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="8">
         <v>1000</v>
       </c>
       <c r="H62" s="1">
@@ -4272,12 +4363,15 @@
       <c r="R62" s="3"/>
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
+      <c r="U62" s="3" t="s">
+        <v>227</v>
+      </c>
       <c r="V62" s="3"/>
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="Y62" s="3"/>
+    </row>
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>150</v>
       </c>
@@ -4309,8 +4403,11 @@
         <f t="shared" si="0"/>
         <v>Aziyo Biologics, Inc. AZYO</v>
       </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U63" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>152</v>
       </c>
@@ -4342,17 +4439,20 @@
         <f t="shared" si="0"/>
         <v>Intevac Inc IVAC</v>
       </c>
-      <c r="Y64">
-        <v>0</v>
+      <c r="U64" t="s">
+        <v>229</v>
       </c>
       <c r="Z64">
         <v>0</v>
       </c>
       <c r="AA64">
+        <v>0</v>
+      </c>
+      <c r="AB64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>154</v>
       </c>
@@ -4385,7 +4485,7 @@
         <v>Sezzle Inc. SZL.A</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>156</v>
       </c>
@@ -4417,13 +4517,16 @@
         <f t="shared" si="0"/>
         <v>American Equity Investment Life Holding Co AEL</v>
       </c>
-      <c r="Y66">
-        <v>0</v>
+      <c r="U66" t="s">
+        <v>230</v>
       </c>
       <c r="Z66">
         <v>0</v>
       </c>
       <c r="AA66">
+        <v>0</v>
+      </c>
+      <c r="AB66">
         <v>1</v>
       </c>
     </row>
@@ -4441,7 +4544,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:V66">
+  <conditionalFormatting sqref="K3:W66">
     <cfRule type="beginsWith" dxfId="2" priority="1" operator="beginsWith" text="http">
       <formula>LEFT(K3,LEN("http"))="http"</formula>
     </cfRule>
@@ -4452,10 +4555,7 @@
       <formula>LEFT(K3,LEN("w"))="w"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="T7" r:id="rId1" xr:uid="{03C12284-2349-4FD6-A56C-BB259343DEFC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed more date intake / need more data
i hate paywalls and corporate meaningless yap. boutta sign up for a bajillion free trials just to find none of them have the data i want
</commit_message>
<xml_diff>
--- a/failed_log2.xlsx
+++ b/failed_log2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John DeForest\Desktop\stonx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D089A57-722B-40E2-9C80-199603715D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD6FF76-7F6F-4E83-ACE6-20E7B5178A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2208" yWindow="1056" windowWidth="17280" windowHeight="10512" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
+    <workbookView xWindow="38730" yWindow="3615" windowWidth="17280" windowHeight="10515" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
   </bookViews>
   <sheets>
     <sheet name="failed_log2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="245">
   <si>
     <t>ticker</t>
   </si>
@@ -618,9 +619,6 @@
     <t>I g F</t>
   </si>
   <si>
-    <t>https://www.investing.com/equities/capstar-financial-holdings-inc</t>
-  </si>
-  <si>
     <t>https://www.investing.com/equities/hmn-financial-historical-data</t>
   </si>
   <si>
@@ -778,6 +776,48 @@
   </si>
   <si>
     <t>Exists?</t>
+  </si>
+  <si>
+    <t>https://www.investing.com/equities/capstar-financial-holdings-inc-historical-data</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>schmitty</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>W est</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>mph</t>
+  </si>
+  <si>
+    <t>W/kg/mph</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>kJ (kcal)</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1353,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1767,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10141A12-633E-46F9-B8A5-FB31F61A7B2A}">
   <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1855,13 +1895,13 @@
         <v>176</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>177</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="W1" t="s">
         <v>161</v>
@@ -1994,8 +2034,8 @@
       <c r="S3" t="s">
         <v>166</v>
       </c>
-      <c r="U3" t="s">
-        <v>178</v>
+      <c r="U3" s="7" t="s">
+        <v>231</v>
       </c>
       <c r="Z3">
         <v>1</v>
@@ -2133,7 +2173,7 @@
         <v>166</v>
       </c>
       <c r="U5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.3">
@@ -2169,7 +2209,7 @@
         <v>Central Valley Community Bancorp CVCY</v>
       </c>
       <c r="U6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
@@ -2204,8 +2244,8 @@
         <f t="shared" si="0"/>
         <v>Beacon Roofing Supply Inc BECN</v>
       </c>
-      <c r="U7" s="9" t="s">
-        <v>181</v>
+      <c r="U7" t="s">
+        <v>180</v>
       </c>
       <c r="V7" s="7"/>
       <c r="Z7">
@@ -2269,10 +2309,10 @@
         <v>Secureworks Corp SCWX</v>
       </c>
       <c r="S8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -2308,10 +2348,10 @@
         <v>Nextera Energy Partners, LP NEP</v>
       </c>
       <c r="S9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z9" t="s">
         <v>39</v>
@@ -2353,10 +2393,10 @@
         <v>Brightcove Inc BCOV</v>
       </c>
       <c r="S10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Z10">
         <v>1</v>
@@ -2476,10 +2516,10 @@
         <v>Howard Hughes Corp HHC</v>
       </c>
       <c r="S13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="U13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Z13">
         <v>2.5</v>
@@ -2530,7 +2570,7 @@
         <v>166</v>
       </c>
       <c r="U14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Z14">
         <v>0</v>
@@ -2575,7 +2615,7 @@
         <v>Fusion Acquisition Corp. II FSNB</v>
       </c>
       <c r="U15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.3">
@@ -2647,7 +2687,7 @@
         <v>Community Trust Bancorp Inc /Ky/ QGNC</v>
       </c>
       <c r="U17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
@@ -2683,7 +2723,7 @@
         <v>William Penn Bancorporation WMPN</v>
       </c>
       <c r="U18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.3">
@@ -2719,7 +2759,7 @@
         <v>Stronghold Digital Mining, Inc. SDIG</v>
       </c>
       <c r="U19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.3">
@@ -2788,7 +2828,7 @@
         <v>Augmedix, Inc. AUGX</v>
       </c>
       <c r="U21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AD21" t="s">
         <v>65</v>
@@ -2854,10 +2894,10 @@
         <v>166</v>
       </c>
       <c r="U22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.3">
@@ -2926,7 +2966,7 @@
         <v>Ambrx Biopharma Inc. AMAM</v>
       </c>
       <c r="U24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
@@ -2971,7 +3011,7 @@
         <v>166</v>
       </c>
       <c r="U25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.3">
@@ -3007,7 +3047,7 @@
         <v>Joann Inc. JOAN</v>
       </c>
       <c r="U26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.3">
@@ -3142,7 +3182,7 @@
         <v>Safeguard Scientifics Inc SFE</v>
       </c>
       <c r="U30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Z30" t="s">
         <v>84</v>
@@ -3187,7 +3227,7 @@
         <v>Patriot Transportation Holding, Inc. PATI</v>
       </c>
       <c r="U31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.3">
@@ -3304,7 +3344,7 @@
         <v>166</v>
       </c>
       <c r="U34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.3">
@@ -3349,7 +3389,7 @@
         <v>166</v>
       </c>
       <c r="U35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.3">
@@ -3385,7 +3425,7 @@
         <v>Corner Growth Acquisition Corp. COOL</v>
       </c>
       <c r="U36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
@@ -3421,7 +3461,7 @@
         <v>Pardes Biosciences, Inc. PRDS</v>
       </c>
       <c r="U37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
@@ -3490,7 +3530,7 @@
         <v>Malvern Bancorp, Inc. MLVF</v>
       </c>
       <c r="U39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
@@ -3535,7 +3575,7 @@
         <v>166</v>
       </c>
       <c r="U40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
@@ -3604,7 +3644,7 @@
         <v>Curo Group Holdings Corp. CURO</v>
       </c>
       <c r="U42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
@@ -3682,7 +3722,7 @@
         <v>Trailblazer Merger Corp I TBMCU</v>
       </c>
       <c r="U44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
@@ -3718,7 +3758,7 @@
         <v>Codorus Valley Bancorp Inc CVLY</v>
       </c>
       <c r="U45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
@@ -3754,7 +3794,7 @@
         <v>Activision Blizzard, Inc. ATVI</v>
       </c>
       <c r="U46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.3">
@@ -3790,13 +3830,13 @@
         <v>Profrac Holding Corp. PFHC</v>
       </c>
       <c r="U47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
@@ -3832,13 +3872,13 @@
         <v>Glatfelter Corp GLT</v>
       </c>
       <c r="U48" t="s">
+        <v>210</v>
+      </c>
+      <c r="V48" t="s">
         <v>211</v>
       </c>
-      <c r="V48" t="s">
-        <v>212</v>
-      </c>
       <c r="W48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.3">
@@ -3874,7 +3914,7 @@
         <v>Adams Resources &amp; Energy, Inc. AE</v>
       </c>
       <c r="U49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.3">
@@ -3910,7 +3950,7 @@
         <v>Terrascend Corp. TRSSF</v>
       </c>
       <c r="U50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
@@ -3946,7 +3986,7 @@
         <v>Sentinel Energy Services Inc. STNL</v>
       </c>
       <c r="U51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.3">
@@ -3982,7 +4022,7 @@
         <v>Dice Therapeutics, Inc. DICE</v>
       </c>
       <c r="U52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Z52">
         <v>0</v>
@@ -4030,7 +4070,7 @@
         <v>Miromatrix Medical Inc. MIRO</v>
       </c>
       <c r="U53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.3">
@@ -4066,7 +4106,7 @@
         <v>Absolute Software Corp ABST</v>
       </c>
       <c r="U54" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.3">
@@ -4135,7 +4175,7 @@
         <v>Paratek Pharmaceuticals, Inc. PRTK</v>
       </c>
       <c r="U56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.3">
@@ -4171,7 +4211,7 @@
         <v>Chimerix Inc CMRX</v>
       </c>
       <c r="U57" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Z57">
         <v>0</v>
@@ -4216,7 +4256,7 @@
         <v>Fisker Inc./de FSR</v>
       </c>
       <c r="U58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.3">
@@ -4285,7 +4325,7 @@
         <v>Air Transport Services Group, Inc. ATSG</v>
       </c>
       <c r="U60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.3">
@@ -4321,7 +4361,7 @@
         <v>U-Haul Holding Co /Nv/ UHALU</v>
       </c>
       <c r="U61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.3">
@@ -4364,7 +4404,7 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
       <c r="U62" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="V62" s="3"/>
       <c r="W62" s="3"/>
@@ -4404,7 +4444,7 @@
         <v>Aziyo Biologics, Inc. AZYO</v>
       </c>
       <c r="U63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
@@ -4440,7 +4480,7 @@
         <v>Intevac Inc IVAC</v>
       </c>
       <c r="U64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Z64">
         <v>0</v>
@@ -4518,7 +4558,7 @@
         <v>American Equity Investment Life Holding Co AEL</v>
       </c>
       <c r="U66" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Z66">
         <v>0</v>
@@ -4555,7 +4595,159 @@
       <formula>LEFT(K3,LEN("w"))="w"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="U3" r:id="rId1" xr:uid="{5C97046D-313C-4638-BC07-DFED2E8ED957}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB78E7F-A549-4A74-B8CE-A108A508C02A}">
+  <dimension ref="A8:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" t="s">
+        <v>237</v>
+      </c>
+      <c r="F8" t="s">
+        <v>238</v>
+      </c>
+      <c r="G8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H8" t="s">
+        <v>238</v>
+      </c>
+      <c r="I8" t="s">
+        <v>240</v>
+      </c>
+      <c r="J8" t="s">
+        <v>241</v>
+      </c>
+      <c r="K8" t="s">
+        <v>242</v>
+      </c>
+      <c r="M8" t="s">
+        <v>243</v>
+      </c>
+      <c r="N8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9">
+        <v>165</v>
+      </c>
+      <c r="C9">
+        <f>B9/2.2</f>
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>3.64</v>
+      </c>
+      <c r="E9">
+        <v>243</v>
+      </c>
+      <c r="F9">
+        <v>43</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <f>F9+G9/60</f>
+        <v>43.05</v>
+      </c>
+      <c r="I9">
+        <f>H9/60</f>
+        <v>0.71749999999999992</v>
+      </c>
+      <c r="J9">
+        <f>D9/I9</f>
+        <v>5.073170731707318</v>
+      </c>
+      <c r="K9">
+        <f>E9/J9/C9</f>
+        <v>0.63865384615384602</v>
+      </c>
+      <c r="M9">
+        <f>E9*H9*60</f>
+        <v>627669</v>
+      </c>
+      <c r="N9">
+        <f>M9/1000</f>
+        <v>627.66899999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10">
+        <f>C10*2.2</f>
+        <v>174.9</v>
+      </c>
+      <c r="C10">
+        <v>79.5</v>
+      </c>
+      <c r="D10">
+        <v>3.64</v>
+      </c>
+      <c r="E10" s="9">
+        <v>303</v>
+      </c>
+      <c r="F10">
+        <v>36</v>
+      </c>
+      <c r="G10">
+        <v>37</v>
+      </c>
+      <c r="H10">
+        <f>F10+G10/60</f>
+        <v>36.616666666666667</v>
+      </c>
+      <c r="I10">
+        <f>H10/60</f>
+        <v>0.61027777777777781</v>
+      </c>
+      <c r="J10">
+        <f>D10/I10</f>
+        <v>5.9644970414201186</v>
+      </c>
+      <c r="K10">
+        <f>E10/C10/J10</f>
+        <v>0.63900119796346211</v>
+      </c>
+      <c r="M10">
+        <f>E10*H10*60</f>
+        <v>665691</v>
+      </c>
+      <c r="N10">
+        <f>M10/1000</f>
+        <v>665.69100000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Urg. back to icom pipeline?
tbh at this point might as well manually download that woulda been faster smh my head.
</commit_message>
<xml_diff>
--- a/failed_log2.xlsx
+++ b/failed_log2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John DeForest\Desktop\stonx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD6FF76-7F6F-4E83-ACE6-20E7B5178A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85453C72-AD69-4CC2-A8F7-702894ECA6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38730" yWindow="3615" windowWidth="17280" windowHeight="10515" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
   </bookViews>
   <sheets>
     <sheet name="failed_log2" sheetId="1" r:id="rId1"/>
@@ -1807,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10141A12-633E-46F9-B8A5-FB31F61A7B2A}">
   <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Can rip charts now :)
requires manual loc setup and mouse takeover. lol. oh well. #dataordie. do not use barchart_ripper2 it doesnt work
</commit_message>
<xml_diff>
--- a/failed_log2.xlsx
+++ b/failed_log2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John DeForest\Desktop\stonx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85453C72-AD69-4CC2-A8F7-702894ECA6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CED7CE3-493C-4BFD-90F8-99AFBF7AFF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
+    <workbookView xWindow="30525" yWindow="3450" windowWidth="24600" windowHeight="11925" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
   </bookViews>
   <sheets>
     <sheet name="failed_log2" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,8 @@
     <author>tc={81845068-A864-422B-A307-D209ED86063D}</author>
     <author>tc={87EC06C1-C95E-4B45-B805-4D4BCEE2B9EE}</author>
     <author>tc={41293392-54A1-4296-96FD-EDB13FBD4F4E}</author>
+    <author>John DeForest</author>
+    <author>tc={B1DD0A28-EE6E-42D6-8FC5-EED5B576588F}</author>
     <author>tc={CB4462E8-6D40-43DF-871C-DAA05325856A}</author>
   </authors>
   <commentList>
@@ -68,7 +70,46 @@
     G = google search only, It = investing.com search bar ticker, in = ‘ full name</t>
       </text>
     </comment>
-    <comment ref="G62" authorId="3" shapeId="0" xr:uid="{CB4462E8-6D40-43DF-871C-DAA05325856A}">
+    <comment ref="T22" authorId="3" shapeId="0" xr:uid="{C70B49C7-29E3-4763-A5C6-572A7585F72C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>John DeForest:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FAILED PULL - requires free trial of options see comment
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U22" authorId="4" shapeId="0" xr:uid="{B1DD0A28-EE6E-42D6-8FC5-EED5B576588F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Any of the following sources require fuck ass subscription
+Reply:
+    https://www.marketbeat.com/stocks/NASDAQ/MICS/chart/
+Reply:
+    https://stockinvest.us/stock-price/MICS?from=2019-01-01&amp;to=2025-08-04&amp;page=6
+Reply:
+    Or could build some sort of chart scraper from one of these: 1) https://fintel.io/chart/us/mics or 2) https://www.barchart.com/stocks/quotes/MICS/interactive-chart</t>
+      </text>
+    </comment>
+    <comment ref="G62" authorId="5" shapeId="0" xr:uid="{CB4462E8-6D40-43DF-871C-DAA05325856A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -827,7 +868,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,8 +1017,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1181,6 +1235,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1343,7 +1403,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1354,6 +1414,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1794,6 +1855,37 @@
   <threadedComment ref="Y1" dT="2025-07-31T18:20:10.90" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{41293392-54A1-4296-96FD-EDB13FBD4F4E}">
     <text>G = google search only, It = investing.com search bar ticker, in = ‘ full name</text>
   </threadedComment>
+  <threadedComment ref="U22" dT="2025-08-06T05:13:57.83" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{B1DD0A28-EE6E-42D6-8FC5-EED5B576588F}">
+    <text>Any of the following sources require fuck ass subscription</text>
+  </threadedComment>
+  <threadedComment ref="U22" dT="2025-08-06T05:14:06.36" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{2BE39E21-D65D-4FC4-A3B1-21B83B9E75FF}" parentId="{B1DD0A28-EE6E-42D6-8FC5-EED5B576588F}">
+    <text>https://www.marketbeat.com/stocks/NASDAQ/MICS/chart/</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>2329312997</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="52" url="https://www.marketbeat.com/stocks/NASDAQ/MICS/chart/"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="U22" dT="2025-08-06T05:14:28.54" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{241381A7-C6F9-4688-AA24-4857B754328F}" parentId="{B1DD0A28-EE6E-42D6-8FC5-EED5B576588F}">
+    <text>https://stockinvest.us/stock-price/MICS?from=2019-01-01&amp;to=2025-08-04&amp;page=6</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>2187967734</xltc2:checksum>
+        <xltc2:hyperlink startIndex="0" length="76" url="https://stockinvest.us/stock-price/MICS?from=2019-01-01&amp;to=2025-08-04&amp;page=6"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="U22" dT="2025-08-06T05:15:00.14" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{2CAB16D7-165F-4E6F-BF8F-3248BFDC5190}" parentId="{B1DD0A28-EE6E-42D6-8FC5-EED5B576588F}">
+    <text>Or could build some sort of chart scraper from one of these: 1) https://fintel.io/chart/us/mics or 2) https://www.barchart.com/stocks/quotes/MICS/interactive-chart</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>351789796</xltc2:checksum>
+        <xltc2:hyperlink startIndex="64" length="31" url="https://fintel.io/chart/us/mics"/>
+        <xltc2:hyperlink startIndex="102" length="61" url="https://www.barchart.com/stocks/quotes/MICS/interactive-chart"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
   <threadedComment ref="G62" dT="2025-08-03T05:02:25.58" personId="{571A1BD7-5BDB-4FF3-A087-C50E31B83295}" id="{CB4462E8-6D40-43DF-871C-DAA05325856A}">
     <text>Double check this manually from the openinsider info...</text>
   </threadedComment>
@@ -1807,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10141A12-633E-46F9-B8A5-FB31F61A7B2A}">
   <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2893,7 +2985,8 @@
       <c r="S22" t="s">
         <v>166</v>
       </c>
-      <c r="U22" t="s">
+      <c r="T22" s="10"/>
+      <c r="U22" s="10" t="s">
         <v>194</v>
       </c>
       <c r="V22" t="s">

</xml_diff>

<commit_message>
tried HPC, ran big OIP pull, csv'd
wowzers. yf limiter. ugh i have 2000 rows to manually find lmfao. gah. i need an intern. or better yet, and incoming summer investment banking analyst
</commit_message>
<xml_diff>
--- a/failed_log2.xlsx
+++ b/failed_log2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John DeForest\Desktop\stonx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF0E0FB-025D-40C2-9039-E551C803EE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EB10AA-440F-4A9B-BD37-7B13AB777F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30525" yWindow="3450" windowWidth="24600" windowHeight="11925" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
+    <workbookView xWindow="0" yWindow="384" windowWidth="23232" windowHeight="11928" xr2:uid="{B9A727A3-84CD-4226-9DF2-A39C96F8305B}"/>
   </bookViews>
   <sheets>
     <sheet name="failed_log2" sheetId="1" r:id="rId1"/>
@@ -1899,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10141A12-633E-46F9-B8A5-FB31F61A7B2A}">
   <dimension ref="A1:AH66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>